<commit_message>
Update exe and server build
</commit_message>
<xml_diff>
--- a/slip_gaji.xlsx
+++ b/slip_gaji.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT-Ananda\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT-Ananda\Documents\react-folder\slip-gaji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240353B3-D7DD-4A57-BDF7-1C56B39624F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D664DC-2474-4911-8EA0-5357CC30BA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E32B845-9068-405A-8C8B-3C3AB2660D08}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{7E32B845-9068-405A-8C8B-3C3AB2660D08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Data Gaji Bulan</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t>Kp. Irian Bekasi</t>
+  </si>
+  <si>
+    <t>NURA ESTA SAPITRI</t>
+  </si>
+  <si>
+    <t>PT2025</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>6289669326911</t>
   </si>
 </sst>
 </file>
@@ -427,6 +439,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -441,15 +462,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,13 +779,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600F822-DD86-4B7F-8DF4-D1492BED4790}">
   <dimension ref="A1:S1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
@@ -790,14 +802,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="27" t="s">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="26"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -814,10 +826,10 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -838,10 +850,10 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="3" t="s">
         <v>39</v>
       </c>
@@ -862,10 +874,10 @@
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="3" t="s">
         <v>41</v>
       </c>
@@ -886,20 +898,20 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="3">
         <f>COUNT(A9:A1010)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -920,21 +932,21 @@
       <c r="C6" s="16"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="22" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
     </row>
@@ -993,7 +1005,7 @@
       <c r="R7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="S7" s="25"/>
+      <c r="S7" s="20"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
@@ -1232,36 +1244,64 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="A12" s="7">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="10">
+        <v>4750000</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2100000</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="I12" s="10">
+        <v>500000</v>
+      </c>
+      <c r="J12" s="10">
+        <v>300000</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
       <c r="L12" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8650000</v>
       </c>
       <c r="M12" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+        <v>712500</v>
+      </c>
+      <c r="N12" s="10">
+        <v>90000</v>
+      </c>
+      <c r="O12" s="10">
+        <v>1250000</v>
+      </c>
       <c r="P12" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2052500</v>
       </c>
       <c r="Q12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="12"/>
+        <v>6597500</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>

</xml_diff>

<commit_message>
fix be and fe
</commit_message>
<xml_diff>
--- a/slip_gaji.xlsx
+++ b/slip_gaji.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT-Ananda\Documents\react-folder\slip-gaji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D664DC-2474-4911-8EA0-5357CC30BA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB04B83-013E-476A-B592-44B0104FC273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{7E32B845-9068-405A-8C8B-3C3AB2660D08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E32B845-9068-405A-8C8B-3C3AB2660D08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Data Gaji Bulan</t>
   </si>
   <si>
     <t>Nama Bendahara</t>
-  </si>
-  <si>
-    <t>M. FATIH</t>
   </si>
   <si>
     <t>Jumlah Karyawan</t>
@@ -84,12 +81,6 @@
     <t>TUNJANGAN LAIN-LAIN</t>
   </si>
   <si>
-    <t>LEMBUR</t>
-  </si>
-  <si>
-    <t>THR</t>
-  </si>
-  <si>
     <t>JML PENDAPATAN</t>
   </si>
   <si>
@@ -105,56 +96,11 @@
     <t>JML POTONGAN</t>
   </si>
   <si>
-    <t>ABDUL HAKIM</t>
-  </si>
-  <si>
-    <t>EN001</t>
-  </si>
-  <si>
-    <t>ENGINEERING</t>
-  </si>
-  <si>
-    <t>111222333444</t>
-  </si>
-  <si>
-    <t>6281234567890</t>
-  </si>
-  <si>
-    <t>ZAARA AQILLA</t>
-  </si>
-  <si>
-    <t>PM001</t>
-  </si>
-  <si>
-    <t>PROJECT MANAGER</t>
-  </si>
-  <si>
-    <t>222333444555</t>
-  </si>
-  <si>
-    <t>FAIZAR KHAIRI</t>
-  </si>
-  <si>
-    <t>QC001</t>
-  </si>
-  <si>
-    <t>QUALITY CONTROL</t>
-  </si>
-  <si>
-    <t>333444555666</t>
-  </si>
-  <si>
-    <t>Maret 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">No Whatsapp
 </t>
   </si>
   <si>
     <t>Nama Perusahaan</t>
-  </si>
-  <si>
-    <t>RS. Ananda Bekasi</t>
   </si>
   <si>
     <t>Kota</t>
@@ -169,16 +115,25 @@
     <t>Kp. Irian Bekasi</t>
   </si>
   <si>
-    <t>NURA ESTA SAPITRI</t>
+    <t>Febriansyah</t>
   </si>
   <si>
-    <t>PT2025</t>
+    <t>Zeeva</t>
   </si>
   <si>
-    <t>IT</t>
+    <t>Kwala Creative</t>
   </si>
   <si>
-    <t>6289669326911</t>
+    <t>Marketting</t>
+  </si>
+  <si>
+    <t>April 2025</t>
+  </si>
+  <si>
+    <t>3698563</t>
+  </si>
+  <si>
+    <t>62895700355535</t>
   </si>
 </sst>
 </file>
@@ -445,7 +400,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -779,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4600F822-DD86-4B7F-8DF4-D1492BED4790}">
   <dimension ref="A1:S1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +762,7 @@
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="2"/>
@@ -831,7 +786,7 @@
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
@@ -851,11 +806,11 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2"/>
@@ -875,11 +830,11 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
@@ -899,19 +854,19 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="3">
         <f>COUNT(A9:A1010)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -933,7 +888,7 @@
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
       <c r="F6" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
@@ -942,7 +897,7 @@
       <c r="K6" s="24"/>
       <c r="L6" s="24"/>
       <c r="M6" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N6" s="26"/>
       <c r="O6" s="26"/>
@@ -952,58 +907,54 @@
     </row>
     <row r="7" spans="1:19" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="C7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="D7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>8</v>
-      </c>
       <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="N7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="P7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="Q7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="R7" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="S7" s="20"/>
     </row>
@@ -1068,240 +1019,152 @@
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="C9" s="7">
+        <v>36956325</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F9" s="10">
-        <v>4500000</v>
+        <v>6500000</v>
       </c>
       <c r="G9" s="10">
-        <v>2100000</v>
+        <v>500000</v>
       </c>
       <c r="H9" s="10">
-        <v>1000000</v>
+        <v>300000</v>
       </c>
       <c r="I9" s="10">
-        <v>500000</v>
-      </c>
-      <c r="J9" s="10">
-        <v>550000</v>
-      </c>
-      <c r="K9" s="10">
-        <v>0</v>
-      </c>
+        <v>800000</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
       <c r="L9" s="11">
         <f>SUM(F9:K9)</f>
-        <v>8650000</v>
+        <v>8100000</v>
       </c>
       <c r="M9" s="10">
-        <f>15%*F9</f>
-        <v>675000</v>
+        <f t="shared" ref="M9:M73" si="0">15%*F9</f>
+        <v>975000</v>
       </c>
       <c r="N9" s="10">
-        <v>90000</v>
+        <v>250000</v>
       </c>
       <c r="O9" s="10">
-        <v>1150000</v>
+        <v>100000</v>
       </c>
       <c r="P9" s="11">
         <f>SUM(M9:O9)</f>
-        <v>1915000</v>
+        <v>1325000</v>
       </c>
       <c r="Q9" s="11">
         <f>L9-P9</f>
-        <v>6735000</v>
+        <v>6775000</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>2</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="10">
-        <v>5000000</v>
-      </c>
-      <c r="G10" s="10">
-        <v>2250000</v>
-      </c>
-      <c r="H10" s="10">
-        <v>1250000</v>
-      </c>
-      <c r="I10" s="10">
-        <v>500000</v>
-      </c>
-      <c r="J10" s="10">
-        <v>0</v>
-      </c>
-      <c r="K10" s="10">
-        <v>0</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
       <c r="L10" s="11">
-        <f t="shared" ref="L10:L73" si="0">SUM(F10:K10)</f>
-        <v>9000000</v>
+        <f t="shared" ref="L10:L73" si="1">SUM(F10:K10)</f>
+        <v>0</v>
       </c>
       <c r="M10" s="10">
-        <f t="shared" ref="M10:M73" si="1">15%*F10</f>
-        <v>750000</v>
-      </c>
-      <c r="N10" s="10">
-        <v>90000</v>
-      </c>
-      <c r="O10" s="10">
-        <v>1000000</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
       <c r="P10" s="11">
         <f t="shared" ref="P10:P73" si="2">SUM(M10:O10)</f>
-        <v>1840000</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="11">
         <f t="shared" ref="Q10:Q73" si="3">L10-P10</f>
-        <v>7160000</v>
-      </c>
-      <c r="R10" s="12" t="s">
-        <v>27</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R10" s="12"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>3</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="10">
-        <v>4750000</v>
-      </c>
-      <c r="G11" s="10">
-        <v>2100000</v>
-      </c>
-      <c r="H11" s="10">
-        <v>1000000</v>
-      </c>
-      <c r="I11" s="10">
-        <v>500000</v>
-      </c>
-      <c r="J11" s="10">
-        <v>300000</v>
-      </c>
-      <c r="K11" s="10">
-        <v>0</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
       <c r="L11" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
         <f t="shared" si="0"/>
-        <v>8650000</v>
-      </c>
-      <c r="M11" s="10">
-        <f t="shared" si="1"/>
-        <v>712500</v>
-      </c>
-      <c r="N11" s="10">
-        <v>90000</v>
-      </c>
-      <c r="O11" s="10">
-        <v>1250000</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
       <c r="P11" s="11">
         <f t="shared" si="2"/>
-        <v>2052500</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="11">
         <f t="shared" si="3"/>
-        <v>6597500</v>
-      </c>
-      <c r="R11" s="12" t="s">
-        <v>27</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R11" s="12"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>4</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="10">
-        <v>4750000</v>
-      </c>
-      <c r="G12" s="10">
-        <v>2100000</v>
-      </c>
-      <c r="H12" s="10">
-        <v>1000000</v>
-      </c>
-      <c r="I12" s="10">
-        <v>500000</v>
-      </c>
-      <c r="J12" s="10">
-        <v>300000</v>
-      </c>
-      <c r="K12" s="10">
-        <v>0</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
       <c r="L12" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
         <f t="shared" si="0"/>
-        <v>8650000</v>
-      </c>
-      <c r="M12" s="10">
-        <f t="shared" si="1"/>
-        <v>712500</v>
-      </c>
-      <c r="N12" s="10">
-        <v>90000</v>
-      </c>
-      <c r="O12" s="10">
-        <v>1250000</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
       <c r="P12" s="11">
         <f t="shared" si="2"/>
-        <v>2052500</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="11">
         <f t="shared" si="3"/>
-        <v>6597500</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>47</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R12" s="12"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
@@ -1316,11 +1179,11 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N13" s="10"/>
@@ -1348,11 +1211,11 @@
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N14" s="10"/>
@@ -1380,11 +1243,11 @@
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N15" s="10"/>
@@ -1412,11 +1275,11 @@
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N16" s="10"/>
@@ -1444,11 +1307,11 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N17" s="10"/>
@@ -1476,11 +1339,11 @@
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N18" s="10"/>
@@ -1508,11 +1371,11 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N19" s="10"/>
@@ -1540,11 +1403,11 @@
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N20" s="10"/>
@@ -1572,11 +1435,11 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N21" s="10"/>
@@ -1604,11 +1467,11 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N22" s="10"/>
@@ -1636,11 +1499,11 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N23" s="10"/>
@@ -1668,11 +1531,11 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N24" s="10"/>
@@ -1700,11 +1563,11 @@
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="L25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N25" s="10"/>
@@ -1732,11 +1595,11 @@
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N26" s="10"/>
@@ -1764,11 +1627,11 @@
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
       <c r="L27" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N27" s="10"/>
@@ -1796,11 +1659,11 @@
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M28" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N28" s="10"/>
@@ -1828,11 +1691,11 @@
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N29" s="10"/>
@@ -1860,11 +1723,11 @@
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
       <c r="L30" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N30" s="10"/>
@@ -1892,11 +1755,11 @@
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N31" s="10"/>
@@ -1924,11 +1787,11 @@
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N32" s="10"/>
@@ -1956,11 +1819,11 @@
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
       <c r="L33" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N33" s="10"/>
@@ -1988,11 +1851,11 @@
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
       <c r="L34" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N34" s="10"/>
@@ -2020,11 +1883,11 @@
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M35" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N35" s="10"/>
@@ -2052,11 +1915,11 @@
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
       <c r="L36" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N36" s="10"/>
@@ -2084,11 +1947,11 @@
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
       <c r="L37" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M37" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N37" s="10"/>
@@ -2116,11 +1979,11 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
       <c r="L38" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M38" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N38" s="10"/>
@@ -2148,11 +2011,11 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
       <c r="L39" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N39" s="10"/>
@@ -2180,11 +2043,11 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
       <c r="L40" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M40" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N40" s="10"/>
@@ -2212,11 +2075,11 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
       <c r="L41" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N41" s="10"/>
@@ -2244,11 +2107,11 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
       <c r="L42" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M42" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N42" s="10"/>
@@ -2276,11 +2139,11 @@
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
       <c r="L43" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M43" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N43" s="10"/>
@@ -2308,11 +2171,11 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
       <c r="L44" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N44" s="10"/>
@@ -2340,11 +2203,11 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
       <c r="L45" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N45" s="10"/>
@@ -2372,11 +2235,11 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
       <c r="L46" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M46" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N46" s="10"/>
@@ -2404,11 +2267,11 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
       <c r="L47" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M47" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M47" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N47" s="10"/>
@@ -2436,11 +2299,11 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
       <c r="L48" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N48" s="10"/>
@@ -2468,11 +2331,11 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
       <c r="L49" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M49" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N49" s="10"/>
@@ -2500,11 +2363,11 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
       <c r="L50" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M50" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M50" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N50" s="10"/>
@@ -2532,11 +2395,11 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
       <c r="L51" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M51" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M51" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N51" s="10"/>
@@ -2564,11 +2427,11 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
       <c r="L52" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M52" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M52" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N52" s="10"/>
@@ -2596,11 +2459,11 @@
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
       <c r="L53" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M53" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N53" s="10"/>
@@ -2628,11 +2491,11 @@
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
       <c r="L54" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M54" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N54" s="10"/>
@@ -2660,11 +2523,11 @@
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
       <c r="L55" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M55" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N55" s="10"/>
@@ -2692,11 +2555,11 @@
       <c r="J56" s="10"/>
       <c r="K56" s="10"/>
       <c r="L56" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M56" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N56" s="10"/>
@@ -2724,11 +2587,11 @@
       <c r="J57" s="10"/>
       <c r="K57" s="10"/>
       <c r="L57" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M57" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M57" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N57" s="10"/>
@@ -2756,11 +2619,11 @@
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
       <c r="L58" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M58" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M58" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N58" s="10"/>
@@ -2788,11 +2651,11 @@
       <c r="J59" s="10"/>
       <c r="K59" s="10"/>
       <c r="L59" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M59" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M59" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N59" s="10"/>
@@ -2820,11 +2683,11 @@
       <c r="J60" s="10"/>
       <c r="K60" s="10"/>
       <c r="L60" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M60" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M60" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N60" s="10"/>
@@ -2852,11 +2715,11 @@
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
       <c r="L61" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M61" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M61" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N61" s="10"/>
@@ -2884,11 +2747,11 @@
       <c r="J62" s="10"/>
       <c r="K62" s="10"/>
       <c r="L62" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M62" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M62" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N62" s="10"/>
@@ -2916,11 +2779,11 @@
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
       <c r="L63" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M63" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M63" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N63" s="10"/>
@@ -2948,11 +2811,11 @@
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
       <c r="L64" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M64" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M64" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N64" s="10"/>
@@ -2980,11 +2843,11 @@
       <c r="J65" s="10"/>
       <c r="K65" s="10"/>
       <c r="L65" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M65" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M65" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N65" s="10"/>
@@ -3012,11 +2875,11 @@
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
       <c r="L66" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M66" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M66" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N66" s="10"/>
@@ -3044,11 +2907,11 @@
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
       <c r="L67" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M67" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M67" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N67" s="10"/>
@@ -3076,11 +2939,11 @@
       <c r="J68" s="10"/>
       <c r="K68" s="10"/>
       <c r="L68" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M68" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M68" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N68" s="10"/>
@@ -3108,11 +2971,11 @@
       <c r="J69" s="10"/>
       <c r="K69" s="10"/>
       <c r="L69" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M69" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M69" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N69" s="10"/>
@@ -3140,11 +3003,11 @@
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
       <c r="L70" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M70" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M70" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N70" s="10"/>
@@ -3172,11 +3035,11 @@
       <c r="J71" s="10"/>
       <c r="K71" s="10"/>
       <c r="L71" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M71" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M71" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N71" s="10"/>
@@ -3204,11 +3067,11 @@
       <c r="J72" s="10"/>
       <c r="K72" s="10"/>
       <c r="L72" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M72" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M72" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N72" s="10"/>
@@ -3236,11 +3099,11 @@
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
       <c r="L73" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M73" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M73" s="10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N73" s="10"/>

</xml_diff>